<commit_message>
Use read-only openpyxl workbook to read form definition
</commit_message>
<xml_diff>
--- a/tests/example_xls/group.xlsx
+++ b/tests/example_xls/group.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{62F363D5-98BC-4F6C-B977-FD007F1C4253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B259AC39-EDB2-A749-9594-051521C730BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="16170" tabRatio="60"/>
+    <workbookView xWindow="9620" yWindow="5420" windowWidth="28780" windowHeight="16180" tabRatio="60" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -77,7 +68,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -512,22 +503,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C83"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="38" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="78.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="78.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +529,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -549,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -560,7 +551,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -571,7 +562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -582,71 +573,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:3" ht="76.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="102" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="76.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="76.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="140.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="51" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="76.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="63.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="38.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777772" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>

</xml_diff>